<commit_message>
Update CV on RDP
</commit_message>
<xml_diff>
--- a/UIAutomationRDP/Transaction.xlsx
+++ b/UIAutomationRDP/Transaction.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hongphucvi\Documents\GitHub\RPA\UIAutomationRDP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C1762F-8D79-4F9F-9ED3-D5BD932BF823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01BCA971-35B4-4CAD-9932-C1B6B587968E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="13680" windowHeight="7245" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -409,7 +409,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>430030</v>
+        <v>197707</v>
       </c>
     </row>
   </sheetData>

</xml_diff>